<commit_message>
CSV support added,example In/ Output : Testfiles
</commit_message>
<xml_diff>
--- a/Kontaktdruck_Tool_Richard_F_Vorlage.xlsx
+++ b/Kontaktdruck_Tool_Richard_F_Vorlage.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C132386-4CF9-0A43-94CF-687BC29785E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81FBAB4-E62E-0D46-9B5B-942D54C91C0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,79 +388,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>389283</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>106846</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>475008</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>4555</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="[0]!Makro1" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rechteck 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12647544" y="520976"/>
-          <a:ext cx="1311551" cy="552036"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent5"/>
-        </a:fillRef>
-        <a:effectRef idx="3">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1800" b="1">
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Macro</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -5708,6 +5635,5 @@
   <printOptions gridLines="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>